<commit_message>
package int test 1
</commit_message>
<xml_diff>
--- a/calc/files/parcel_int.xlsx
+++ b/calc/files/parcel_int.xlsx
@@ -1792,7 +1792,7 @@
   <cellStyleXfs count="1">
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="1" numFmtId="1000" quotePrefix="false"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="1" numFmtId="1000" quotePrefix="false"/>
     <xf applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="2" fontId="1" numFmtId="1000" quotePrefix="false"/>
     <xf applyAlignment="true" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="2" fontId="1" numFmtId="1000" quotePrefix="false">
@@ -1892,7 +1892,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="4" fillId="2" fontId="5" numFmtId="1000" quotePrefix="false"/>
-    <xf applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="4" fillId="2" fontId="1" numFmtId="1000" quotePrefix="false"/>
     <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="12" fillId="2" fontId="1" numFmtId="1007" quotePrefix="false">
       <alignment vertical="center"/>
     </xf>
@@ -6687,7 +6686,7 @@
       <c r="B161" s="17" t="s">
         <v>316</v>
       </c>
-      <c r="C161" s="39" t="s">
+      <c r="C161" s="36" t="s">
         <v>317</v>
       </c>
       <c r="D161" s="25" t="n">
@@ -8735,11 +8734,11 @@
       <c r="H231" s="26" t="n">
         <v>17.4</v>
       </c>
-      <c r="I231" s="40" t="s">
+      <c r="I231" s="39" t="s">
         <v>458</v>
       </c>
-      <c r="J231" s="41" t="n"/>
-      <c r="K231" s="42" t="s">
+      <c r="J231" s="40" t="n"/>
+      <c r="K231" s="41" t="s">
         <v>459</v>
       </c>
       <c r="L231" s="3" t="n"/>
@@ -8792,7 +8791,7 @@
       <c r="A1" s="8" t="s">
         <v>460</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="42" t="s">
         <v>461</v>
       </c>
       <c r="C1" s="8" t="s">
@@ -8804,40 +8803,40 @@
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">222</f>
         <v>222</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="43" t="s">
         <v>463</v>
       </c>
-      <c r="C2" s="45" t="s"/>
+      <c r="C2" s="44" t="s"/>
     </row>
     <row customHeight="true" ht="26.4500007629395" outlineLevel="0" r="3">
       <c r="A3" s="17" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">A2+1</f>
         <v>223</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="45" t="s">
         <v>464</v>
       </c>
-      <c r="C3" s="47" t="s"/>
+      <c r="C3" s="46" t="s"/>
     </row>
     <row customHeight="true" ht="45.75" outlineLevel="0" r="4">
       <c r="A4" s="17" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">A3+1</f>
         <v>224</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="45" t="s">
         <v>465</v>
       </c>
-      <c r="C4" s="47" t="s"/>
+      <c r="C4" s="46" t="s"/>
     </row>
     <row customHeight="true" ht="50.25" outlineLevel="0" r="5">
       <c r="A5" s="17" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">A4+1</f>
         <v>225</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="47" t="s">
         <v>466</v>
       </c>
-      <c r="C5" s="49" t="n">
+      <c r="C5" s="48" t="n">
         <v>0.03</v>
       </c>
     </row>
@@ -8846,109 +8845,109 @@
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">A5+1</f>
         <v>226</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="47" t="s">
         <v>467</v>
       </c>
-      <c r="C6" s="50" t="n">
+      <c r="C6" s="49" t="n">
         <v>5.85</v>
       </c>
-      <c r="D6" s="51" t="n"/>
+      <c r="D6" s="50" t="n"/>
     </row>
     <row customHeight="true" ht="42" outlineLevel="0" r="7">
       <c r="A7" s="17" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">A6+1</f>
         <v>227</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="43" t="s">
         <v>468</v>
       </c>
-      <c r="C7" s="45" t="s"/>
-      <c r="D7" s="51" t="n"/>
+      <c r="C7" s="44" t="s"/>
+      <c r="D7" s="50" t="n"/>
     </row>
     <row customHeight="true" ht="33.75" outlineLevel="0" r="8">
       <c r="A8" s="17" t="n"/>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="43" t="s">
         <v>469</v>
       </c>
-      <c r="C8" s="45" t="s"/>
-      <c r="D8" s="51" t="n"/>
+      <c r="C8" s="44" t="s"/>
+      <c r="D8" s="50" t="n"/>
     </row>
     <row ht="38.25" outlineLevel="0" r="9">
       <c r="A9" s="17" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">A7+1</f>
         <v>228</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="47" t="s">
         <v>470</v>
       </c>
       <c r="C9" s="34" t="n">
         <v>7.45</v>
       </c>
-      <c r="D9" s="51" t="n"/>
+      <c r="D9" s="50" t="n"/>
     </row>
     <row customHeight="true" ht="39.75" outlineLevel="0" r="10">
       <c r="A10" s="17" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">A9+1</f>
         <v>229</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="45" t="s">
         <v>471</v>
       </c>
-      <c r="C10" s="47" t="s"/>
-      <c r="D10" s="51" t="n"/>
+      <c r="C10" s="46" t="s"/>
+      <c r="D10" s="50" t="n"/>
     </row>
     <row customFormat="true" customHeight="true" ht="57" outlineLevel="0" r="11" s="0">
       <c r="A11" s="17" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">A10+1</f>
         <v>230</v>
       </c>
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="51" t="s">
         <v>472</v>
       </c>
-      <c r="C11" s="53" t="n">
+      <c r="C11" s="52" t="n">
         <v>0.33</v>
       </c>
-      <c r="D11" s="54" t="n"/>
+      <c r="D11" s="53" t="n"/>
     </row>
     <row customHeight="true" ht="27.75" outlineLevel="0" r="12">
       <c r="A12" s="17" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">A11+1</f>
         <v>231</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="45" t="s">
         <v>473</v>
       </c>
-      <c r="C12" s="47" t="s"/>
-      <c r="D12" s="55" t="n"/>
+      <c r="C12" s="46" t="s"/>
+      <c r="D12" s="54" t="n"/>
     </row>
     <row customHeight="true" ht="74.25" outlineLevel="0" r="13">
       <c r="A13" s="17" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">A12+1</f>
         <v>232</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="45" t="s">
         <v>474</v>
       </c>
-      <c r="C13" s="47" t="s"/>
-      <c r="D13" s="55" t="n"/>
+      <c r="C13" s="46" t="s"/>
+      <c r="D13" s="54" t="n"/>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="14">
-      <c r="A14" s="56" t="n"/>
-      <c r="B14" s="57" t="s">
+      <c r="A14" s="55" t="n"/>
+      <c r="B14" s="56" t="s">
         <v>475</v>
       </c>
-      <c r="C14" s="58" t="s"/>
-      <c r="D14" s="55" t="n"/>
+      <c r="C14" s="57" t="s"/>
+      <c r="D14" s="54" t="n"/>
     </row>
     <row customHeight="true" ht="39.5999984741211" outlineLevel="0" r="15">
       <c r="A15" s="17" t="n">
         <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">A13+1</f>
         <v>233</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="45" t="s">
         <v>476</v>
       </c>
-      <c r="C15" s="47" t="s"/>
+      <c r="C15" s="46" t="s"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>